<commit_message>
add "real" data FOLDER to GitHub repository but only "datState" file
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/County Codes to County Names Linkage.xlsx
+++ b/myCBD/myInfo/County Codes to County Names Linkage.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\0.CBD\myCBD\myInfo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8175"/>
   </bookViews>
@@ -657,7 +662,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -962,7 +967,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -970,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,17 +986,16 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1001,29 +1005,29 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>177</v>
+      </c>
       <c r="E1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1033,29 +1037,29 @@
       <c r="C2" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>184</v>
       </c>
       <c r="G2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H2" t="s">
         <v>185</v>
       </c>
       <c r="I2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J2" t="s">
-        <v>184</v>
-      </c>
-      <c r="K2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1065,29 +1069,29 @@
       <c r="C3" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
       <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
         <v>2</v>
       </c>
+      <c r="F3" t="s">
+        <v>184</v>
+      </c>
       <c r="G3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J3" t="s">
-        <v>184</v>
-      </c>
-      <c r="K3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1097,29 +1101,29 @@
       <c r="C4" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
       <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
         <v>3</v>
       </c>
+      <c r="F4" t="s">
+        <v>184</v>
+      </c>
       <c r="G4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J4" t="s">
-        <v>184</v>
-      </c>
-      <c r="K4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1129,29 +1133,29 @@
       <c r="C5" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
       <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
         <v>4</v>
       </c>
+      <c r="F5" t="s">
+        <v>184</v>
+      </c>
       <c r="G5" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J5" t="s">
-        <v>184</v>
-      </c>
-      <c r="K5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1161,29 +1165,29 @@
       <c r="C6" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
       <c r="E6">
-        <v>9</v>
-      </c>
-      <c r="F6">
         <v>5</v>
       </c>
+      <c r="F6" t="s">
+        <v>184</v>
+      </c>
       <c r="G6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J6" t="s">
-        <v>184</v>
-      </c>
-      <c r="K6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1193,29 +1197,29 @@
       <c r="C7" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
       <c r="E7">
-        <v>11</v>
-      </c>
-      <c r="F7">
         <v>6</v>
       </c>
+      <c r="F7" t="s">
+        <v>184</v>
+      </c>
       <c r="G7" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I7" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J7" t="s">
-        <v>184</v>
-      </c>
-      <c r="K7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1225,29 +1229,29 @@
       <c r="C8" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
       <c r="E8">
-        <v>13</v>
-      </c>
-      <c r="F8">
         <v>7</v>
       </c>
+      <c r="F8" t="s">
+        <v>184</v>
+      </c>
       <c r="G8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H8" t="s">
         <v>185</v>
       </c>
       <c r="I8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
-      </c>
-      <c r="K8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1257,29 +1261,29 @@
       <c r="C9" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
       <c r="E9">
-        <v>15</v>
-      </c>
-      <c r="F9">
         <v>8</v>
       </c>
+      <c r="F9" t="s">
+        <v>184</v>
+      </c>
       <c r="G9" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H9" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I9" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J9" t="s">
-        <v>184</v>
-      </c>
-      <c r="K9" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1289,29 +1293,29 @@
       <c r="C10" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
       <c r="E10">
-        <v>17</v>
-      </c>
-      <c r="F10">
         <v>9</v>
       </c>
+      <c r="F10" t="s">
+        <v>184</v>
+      </c>
       <c r="G10" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="H10" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="I10" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J10" t="s">
-        <v>184</v>
-      </c>
-      <c r="K10" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1321,29 +1325,29 @@
       <c r="C11" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
       <c r="E11">
-        <v>19</v>
-      </c>
-      <c r="F11">
         <v>10</v>
       </c>
+      <c r="F11" t="s">
+        <v>184</v>
+      </c>
       <c r="G11" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="H11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I11" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J11" t="s">
-        <v>184</v>
-      </c>
-      <c r="K11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1353,29 +1357,29 @@
       <c r="C12" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
       <c r="E12">
-        <v>21</v>
-      </c>
-      <c r="F12">
         <v>11</v>
       </c>
+      <c r="F12" t="s">
+        <v>184</v>
+      </c>
       <c r="G12" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I12" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J12" t="s">
-        <v>184</v>
-      </c>
-      <c r="K12" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1385,29 +1389,29 @@
       <c r="C13" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="D13">
+        <v>23</v>
+      </c>
       <c r="E13">
-        <v>23</v>
-      </c>
-      <c r="F13">
         <v>12</v>
       </c>
+      <c r="F13" t="s">
+        <v>184</v>
+      </c>
       <c r="G13" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H13" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J13" t="s">
-        <v>184</v>
-      </c>
-      <c r="K13" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1417,29 +1421,29 @@
       <c r="C14" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
       <c r="E14">
-        <v>25</v>
-      </c>
-      <c r="F14">
         <v>13</v>
       </c>
+      <c r="F14" t="s">
+        <v>198</v>
+      </c>
       <c r="G14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I14" t="s">
         <v>198</v>
       </c>
-      <c r="H14" t="s">
-        <v>199</v>
-      </c>
-      <c r="I14" t="s">
-        <v>200</v>
-      </c>
       <c r="J14" t="s">
-        <v>198</v>
-      </c>
-      <c r="K14" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1449,29 +1453,29 @@
       <c r="C15" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="D15">
+        <v>27</v>
+      </c>
       <c r="E15">
-        <v>27</v>
-      </c>
-      <c r="F15">
         <v>14</v>
       </c>
+      <c r="F15" t="s">
+        <v>184</v>
+      </c>
       <c r="G15" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H15" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="I15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J15" t="s">
-        <v>198</v>
-      </c>
-      <c r="K15" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1481,29 +1485,29 @@
       <c r="C16" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="D16">
+        <v>29</v>
+      </c>
       <c r="E16">
-        <v>29</v>
-      </c>
-      <c r="F16">
         <v>15</v>
       </c>
+      <c r="F16" t="s">
+        <v>198</v>
+      </c>
       <c r="G16" t="s">
+        <v>196</v>
+      </c>
+      <c r="H16" t="s">
+        <v>197</v>
+      </c>
+      <c r="I16" t="s">
         <v>198</v>
       </c>
-      <c r="H16" t="s">
-        <v>196</v>
-      </c>
-      <c r="I16" t="s">
-        <v>197</v>
-      </c>
       <c r="J16" t="s">
-        <v>198</v>
-      </c>
-      <c r="K16" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1513,29 +1517,29 @@
       <c r="C17" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="D17">
+        <v>31</v>
+      </c>
       <c r="E17">
-        <v>31</v>
-      </c>
-      <c r="F17">
         <v>16</v>
       </c>
+      <c r="F17" t="s">
+        <v>184</v>
+      </c>
       <c r="G17" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="H17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J17" t="s">
-        <v>198</v>
-      </c>
-      <c r="K17" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1545,29 +1549,29 @@
       <c r="C18" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="D18">
+        <v>33</v>
+      </c>
       <c r="E18">
-        <v>33</v>
-      </c>
-      <c r="F18">
         <v>17</v>
       </c>
+      <c r="F18" t="s">
+        <v>184</v>
+      </c>
       <c r="G18" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H18" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I18" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J18" t="s">
-        <v>184</v>
-      </c>
-      <c r="K18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1577,29 +1581,29 @@
       <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="D19">
+        <v>35</v>
+      </c>
       <c r="E19">
-        <v>35</v>
-      </c>
-      <c r="F19">
         <v>18</v>
       </c>
+      <c r="F19" t="s">
+        <v>184</v>
+      </c>
       <c r="G19" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I19" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J19" t="s">
-        <v>184</v>
-      </c>
-      <c r="K19" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1609,29 +1613,29 @@
       <c r="C20" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="D20">
+        <v>37</v>
+      </c>
       <c r="E20">
-        <v>37</v>
-      </c>
-      <c r="F20">
         <v>19</v>
       </c>
+      <c r="F20" t="s">
+        <v>198</v>
+      </c>
       <c r="G20" t="s">
+        <v>205</v>
+      </c>
+      <c r="H20" t="s">
+        <v>203</v>
+      </c>
+      <c r="I20" t="s">
         <v>198</v>
       </c>
-      <c r="H20" t="s">
-        <v>205</v>
-      </c>
-      <c r="I20" t="s">
-        <v>203</v>
-      </c>
       <c r="J20" t="s">
-        <v>198</v>
-      </c>
-      <c r="K20" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1641,29 +1645,29 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="D21">
+        <v>39</v>
+      </c>
       <c r="E21">
-        <v>39</v>
-      </c>
-      <c r="F21">
         <v>20</v>
       </c>
+      <c r="F21" t="s">
+        <v>184</v>
+      </c>
       <c r="G21" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H21" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="I21" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J21" t="s">
-        <v>184</v>
-      </c>
-      <c r="K21" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1673,29 +1677,29 @@
       <c r="C22" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="D22">
+        <v>41</v>
+      </c>
       <c r="E22">
-        <v>41</v>
-      </c>
-      <c r="F22">
         <v>21</v>
       </c>
+      <c r="F22" t="s">
+        <v>184</v>
+      </c>
       <c r="G22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H22" t="s">
         <v>185</v>
       </c>
       <c r="I22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J22" t="s">
-        <v>184</v>
-      </c>
-      <c r="K22" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1705,29 +1709,29 @@
       <c r="C23" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="D23">
+        <v>43</v>
+      </c>
       <c r="E23">
-        <v>43</v>
-      </c>
-      <c r="F23">
         <v>22</v>
       </c>
+      <c r="F23" t="s">
+        <v>184</v>
+      </c>
       <c r="G23" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H23" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="I23" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J23" t="s">
-        <v>184</v>
-      </c>
-      <c r="K23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -1737,29 +1741,29 @@
       <c r="C24" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="D24">
+        <v>45</v>
+      </c>
       <c r="E24">
-        <v>45</v>
-      </c>
-      <c r="F24">
         <v>23</v>
       </c>
+      <c r="F24" t="s">
+        <v>184</v>
+      </c>
       <c r="G24" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H24" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I24" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J24" t="s">
-        <v>184</v>
-      </c>
-      <c r="K24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1769,29 +1773,29 @@
       <c r="C25" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="D25">
+        <v>47</v>
+      </c>
       <c r="E25">
-        <v>47</v>
-      </c>
-      <c r="F25">
         <v>24</v>
       </c>
+      <c r="F25" t="s">
+        <v>184</v>
+      </c>
       <c r="G25" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="H25" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I25" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J25" t="s">
-        <v>184</v>
-      </c>
-      <c r="K25" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1801,29 +1805,29 @@
       <c r="C26" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="D26">
+        <v>49</v>
+      </c>
       <c r="E26">
-        <v>49</v>
-      </c>
-      <c r="F26">
         <v>25</v>
       </c>
+      <c r="F26" t="s">
+        <v>184</v>
+      </c>
       <c r="G26" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H26" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I26" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J26" t="s">
-        <v>184</v>
-      </c>
-      <c r="K26" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1833,29 +1837,29 @@
       <c r="C27" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="D27">
+        <v>51</v>
+      </c>
       <c r="E27">
-        <v>51</v>
-      </c>
-      <c r="F27">
         <v>26</v>
       </c>
+      <c r="F27" t="s">
+        <v>184</v>
+      </c>
       <c r="G27" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H27" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I27" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J27" t="s">
-        <v>184</v>
-      </c>
-      <c r="K27" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1865,29 +1869,29 @@
       <c r="C28" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="D28">
+        <v>53</v>
+      </c>
       <c r="E28">
-        <v>53</v>
-      </c>
-      <c r="F28">
         <v>27</v>
       </c>
+      <c r="F28" t="s">
+        <v>184</v>
+      </c>
       <c r="G28" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="H28" t="s">
         <v>206</v>
       </c>
       <c r="I28" t="s">
+        <v>184</v>
+      </c>
+      <c r="J28" t="s">
         <v>206</v>
       </c>
-      <c r="J28" t="s">
-        <v>184</v>
-      </c>
-      <c r="K28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1897,29 +1901,29 @@
       <c r="C29" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="D29">
+        <v>55</v>
+      </c>
       <c r="E29">
-        <v>55</v>
-      </c>
-      <c r="F29">
         <v>28</v>
       </c>
+      <c r="F29" t="s">
+        <v>184</v>
+      </c>
       <c r="G29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H29" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="I29" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J29" t="s">
-        <v>184</v>
-      </c>
-      <c r="K29" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1929,29 +1933,29 @@
       <c r="C30" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="D30">
+        <v>57</v>
+      </c>
       <c r="E30">
-        <v>57</v>
-      </c>
-      <c r="F30">
         <v>29</v>
       </c>
+      <c r="F30" t="s">
+        <v>184</v>
+      </c>
       <c r="G30" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I30" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J30" t="s">
-        <v>184</v>
-      </c>
-      <c r="K30" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1961,29 +1965,29 @@
       <c r="C31" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="D31">
+        <v>59</v>
+      </c>
       <c r="E31">
-        <v>59</v>
-      </c>
-      <c r="F31">
         <v>30</v>
       </c>
+      <c r="F31" t="s">
+        <v>198</v>
+      </c>
       <c r="G31" t="s">
+        <v>205</v>
+      </c>
+      <c r="H31" t="s">
+        <v>207</v>
+      </c>
+      <c r="I31" t="s">
         <v>198</v>
       </c>
-      <c r="H31" t="s">
-        <v>205</v>
-      </c>
-      <c r="I31" t="s">
-        <v>207</v>
-      </c>
       <c r="J31" t="s">
-        <v>198</v>
-      </c>
-      <c r="K31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1993,29 +1997,29 @@
       <c r="C32" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="D32">
+        <v>61</v>
+      </c>
       <c r="E32">
-        <v>61</v>
-      </c>
-      <c r="F32">
         <v>31</v>
       </c>
+      <c r="F32" t="s">
+        <v>184</v>
+      </c>
       <c r="G32" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="H32" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="I32" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J32" t="s">
-        <v>184</v>
-      </c>
-      <c r="K32" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2025,29 +2029,29 @@
       <c r="C33" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="D33">
+        <v>63</v>
+      </c>
       <c r="E33">
-        <v>63</v>
-      </c>
-      <c r="F33">
         <v>32</v>
       </c>
+      <c r="F33" t="s">
+        <v>184</v>
+      </c>
       <c r="G33" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H33" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I33" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J33" t="s">
-        <v>184</v>
-      </c>
-      <c r="K33" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2057,29 +2061,29 @@
       <c r="C34" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="D34">
+        <v>65</v>
+      </c>
       <c r="E34">
-        <v>65</v>
-      </c>
-      <c r="F34">
         <v>33</v>
       </c>
+      <c r="F34" t="s">
+        <v>198</v>
+      </c>
       <c r="G34" t="s">
+        <v>208</v>
+      </c>
+      <c r="H34" t="s">
+        <v>202</v>
+      </c>
+      <c r="I34" t="s">
         <v>198</v>
       </c>
-      <c r="H34" t="s">
-        <v>208</v>
-      </c>
-      <c r="I34" t="s">
-        <v>202</v>
-      </c>
       <c r="J34" t="s">
-        <v>198</v>
-      </c>
-      <c r="K34" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2089,29 +2093,29 @@
       <c r="C35" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="D35">
+        <v>67</v>
+      </c>
       <c r="E35">
-        <v>67</v>
-      </c>
-      <c r="F35">
         <v>34</v>
       </c>
+      <c r="F35" t="s">
+        <v>184</v>
+      </c>
       <c r="G35" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="H35" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="I35" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J35" t="s">
-        <v>184</v>
-      </c>
-      <c r="K35" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2121,29 +2125,29 @@
       <c r="C36" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="D36">
+        <v>69</v>
+      </c>
       <c r="E36">
-        <v>69</v>
-      </c>
-      <c r="F36">
         <v>35</v>
       </c>
+      <c r="F36" t="s">
+        <v>184</v>
+      </c>
       <c r="G36" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="H36" t="s">
         <v>206</v>
       </c>
       <c r="I36" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="J36" t="s">
-        <v>184</v>
-      </c>
-      <c r="K36" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>95</v>
       </c>
@@ -2153,29 +2157,29 @@
       <c r="C37" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="D37">
+        <v>71</v>
+      </c>
       <c r="E37">
-        <v>71</v>
-      </c>
-      <c r="F37">
         <v>36</v>
       </c>
+      <c r="F37" t="s">
+        <v>198</v>
+      </c>
       <c r="G37" t="s">
+        <v>208</v>
+      </c>
+      <c r="H37" t="s">
+        <v>202</v>
+      </c>
+      <c r="I37" t="s">
         <v>198</v>
       </c>
-      <c r="H37" t="s">
-        <v>208</v>
-      </c>
-      <c r="I37" t="s">
-        <v>202</v>
-      </c>
       <c r="J37" t="s">
-        <v>198</v>
-      </c>
-      <c r="K37" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2185,29 +2189,29 @@
       <c r="C38" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="D38">
+        <v>73</v>
+      </c>
       <c r="E38">
-        <v>73</v>
-      </c>
-      <c r="F38">
         <v>37</v>
       </c>
+      <c r="F38" t="s">
+        <v>198</v>
+      </c>
       <c r="G38" t="s">
+        <v>199</v>
+      </c>
+      <c r="H38" t="s">
+        <v>200</v>
+      </c>
+      <c r="I38" t="s">
         <v>198</v>
       </c>
-      <c r="H38" t="s">
-        <v>199</v>
-      </c>
-      <c r="I38" t="s">
-        <v>200</v>
-      </c>
       <c r="J38" t="s">
-        <v>198</v>
-      </c>
-      <c r="K38" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2217,29 +2221,29 @@
       <c r="C39" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="D39">
+        <v>75</v>
+      </c>
       <c r="E39">
-        <v>75</v>
-      </c>
-      <c r="F39">
         <v>38</v>
       </c>
+      <c r="F39" t="s">
+        <v>184</v>
+      </c>
       <c r="G39" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H39" t="s">
         <v>185</v>
       </c>
       <c r="I39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J39" t="s">
-        <v>184</v>
-      </c>
-      <c r="K39" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2249,29 +2253,29 @@
       <c r="C40" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="D40">
+        <v>77</v>
+      </c>
       <c r="E40">
-        <v>77</v>
-      </c>
-      <c r="F40">
         <v>39</v>
       </c>
+      <c r="F40" t="s">
+        <v>184</v>
+      </c>
       <c r="G40" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="H40" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I40" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J40" t="s">
-        <v>184</v>
-      </c>
-      <c r="K40" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2281,29 +2285,29 @@
       <c r="C41" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="D41">
+        <v>79</v>
+      </c>
       <c r="E41">
-        <v>79</v>
-      </c>
-      <c r="F41">
         <v>40</v>
       </c>
+      <c r="F41" t="s">
+        <v>198</v>
+      </c>
       <c r="G41" t="s">
+        <v>206</v>
+      </c>
+      <c r="H41" t="s">
+        <v>210</v>
+      </c>
+      <c r="I41" t="s">
         <v>198</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>206</v>
       </c>
-      <c r="I41" t="s">
-        <v>210</v>
-      </c>
-      <c r="J41" t="s">
-        <v>198</v>
-      </c>
-      <c r="K41" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2313,29 +2317,29 @@
       <c r="C42" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="D42">
+        <v>81</v>
+      </c>
       <c r="E42">
-        <v>81</v>
-      </c>
-      <c r="F42">
         <v>41</v>
       </c>
+      <c r="F42" t="s">
+        <v>184</v>
+      </c>
       <c r="G42" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H42" t="s">
         <v>185</v>
       </c>
       <c r="I42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J42" t="s">
-        <v>184</v>
-      </c>
-      <c r="K42" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2345,29 +2349,29 @@
       <c r="C43" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="D43">
+        <v>83</v>
+      </c>
       <c r="E43">
-        <v>83</v>
-      </c>
-      <c r="F43">
         <v>42</v>
       </c>
+      <c r="F43" t="s">
+        <v>198</v>
+      </c>
       <c r="G43" t="s">
+        <v>206</v>
+      </c>
+      <c r="H43" t="s">
+        <v>210</v>
+      </c>
+      <c r="I43" t="s">
         <v>198</v>
       </c>
-      <c r="H43" t="s">
+      <c r="J43" t="s">
         <v>206</v>
       </c>
-      <c r="I43" t="s">
-        <v>210</v>
-      </c>
-      <c r="J43" t="s">
-        <v>198</v>
-      </c>
-      <c r="K43" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2377,29 +2381,29 @@
       <c r="C44" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="D44">
+        <v>85</v>
+      </c>
       <c r="E44">
-        <v>85</v>
-      </c>
-      <c r="F44">
         <v>43</v>
       </c>
+      <c r="F44" t="s">
+        <v>184</v>
+      </c>
       <c r="G44" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H44" t="s">
         <v>185</v>
       </c>
       <c r="I44" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J44" t="s">
-        <v>184</v>
-      </c>
-      <c r="K44" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2409,29 +2413,29 @@
       <c r="C45" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="D45">
+        <v>87</v>
+      </c>
       <c r="E45">
-        <v>87</v>
-      </c>
-      <c r="F45">
         <v>44</v>
       </c>
+      <c r="F45" t="s">
+        <v>184</v>
+      </c>
       <c r="G45" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="H45" t="s">
         <v>206</v>
       </c>
       <c r="I45" t="s">
+        <v>184</v>
+      </c>
+      <c r="J45" t="s">
         <v>206</v>
       </c>
-      <c r="J45" t="s">
-        <v>184</v>
-      </c>
-      <c r="K45" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2441,29 +2445,29 @@
       <c r="C46" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="D46">
+        <v>89</v>
+      </c>
       <c r="E46">
-        <v>89</v>
-      </c>
-      <c r="F46">
         <v>45</v>
       </c>
+      <c r="F46" t="s">
+        <v>184</v>
+      </c>
       <c r="G46" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I46" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J46" t="s">
-        <v>184</v>
-      </c>
-      <c r="K46" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2473,29 +2477,29 @@
       <c r="C47" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="D47">
+        <v>91</v>
+      </c>
       <c r="E47">
-        <v>91</v>
-      </c>
-      <c r="F47">
         <v>46</v>
       </c>
+      <c r="F47" t="s">
+        <v>184</v>
+      </c>
       <c r="G47" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H47" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I47" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J47" t="s">
-        <v>184</v>
-      </c>
-      <c r="K47" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2505,29 +2509,29 @@
       <c r="C48" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="D48">
+        <v>93</v>
+      </c>
       <c r="E48">
-        <v>93</v>
-      </c>
-      <c r="F48">
         <v>47</v>
       </c>
+      <c r="F48" t="s">
+        <v>184</v>
+      </c>
       <c r="G48" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H48" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I48" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J48" t="s">
-        <v>184</v>
-      </c>
-      <c r="K48" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2537,29 +2541,29 @@
       <c r="C49" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="D49">
+        <v>95</v>
+      </c>
       <c r="E49">
-        <v>95</v>
-      </c>
-      <c r="F49">
         <v>48</v>
       </c>
+      <c r="F49" t="s">
+        <v>184</v>
+      </c>
       <c r="G49" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H49" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="I49" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J49" t="s">
-        <v>184</v>
-      </c>
-      <c r="K49" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2569,29 +2573,29 @@
       <c r="C50" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="D50">
+        <v>97</v>
+      </c>
       <c r="E50">
-        <v>97</v>
-      </c>
-      <c r="F50">
         <v>49</v>
       </c>
+      <c r="F50" t="s">
+        <v>184</v>
+      </c>
       <c r="G50" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H50" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="I50" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J50" t="s">
-        <v>184</v>
-      </c>
-      <c r="K50" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2601,29 +2605,29 @@
       <c r="C51" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="D51">
+        <v>99</v>
+      </c>
       <c r="E51">
-        <v>99</v>
-      </c>
-      <c r="F51">
         <v>50</v>
       </c>
+      <c r="F51" t="s">
+        <v>184</v>
+      </c>
       <c r="G51" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="H51" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I51" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J51" t="s">
-        <v>184</v>
-      </c>
-      <c r="K51" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2633,29 +2637,29 @@
       <c r="C52" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="D52">
+        <v>101</v>
+      </c>
       <c r="E52">
-        <v>101</v>
-      </c>
-      <c r="F52">
         <v>51</v>
       </c>
+      <c r="F52" t="s">
+        <v>184</v>
+      </c>
       <c r="G52" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H52" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I52" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J52" t="s">
-        <v>184</v>
-      </c>
-      <c r="K52" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2665,29 +2669,29 @@
       <c r="C53" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="D53">
+        <v>103</v>
+      </c>
       <c r="E53">
-        <v>103</v>
-      </c>
-      <c r="F53">
         <v>52</v>
       </c>
+      <c r="F53" t="s">
+        <v>184</v>
+      </c>
       <c r="G53" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H53" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I53" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J53" t="s">
-        <v>184</v>
-      </c>
-      <c r="K53" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2697,29 +2701,29 @@
       <c r="C54" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="D54">
+        <v>105</v>
+      </c>
       <c r="E54">
-        <v>105</v>
-      </c>
-      <c r="F54">
         <v>53</v>
       </c>
+      <c r="F54" t="s">
+        <v>184</v>
+      </c>
       <c r="G54" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H54" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I54" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J54" t="s">
-        <v>184</v>
-      </c>
-      <c r="K54" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2729,29 +2733,29 @@
       <c r="C55" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="D55">
+        <v>107</v>
+      </c>
       <c r="E55">
-        <v>107</v>
-      </c>
-      <c r="F55">
         <v>54</v>
       </c>
+      <c r="F55" t="s">
+        <v>184</v>
+      </c>
       <c r="G55" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="H55" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I55" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J55" t="s">
-        <v>198</v>
-      </c>
-      <c r="K55" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2761,29 +2765,29 @@
       <c r="C56" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="D56">
+        <v>109</v>
+      </c>
       <c r="E56">
-        <v>109</v>
-      </c>
-      <c r="F56">
         <v>55</v>
       </c>
+      <c r="F56" t="s">
+        <v>184</v>
+      </c>
       <c r="G56" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H56" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I56" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J56" t="s">
-        <v>184</v>
-      </c>
-      <c r="K56" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2793,29 +2797,29 @@
       <c r="C57" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="D57">
+        <v>111</v>
+      </c>
       <c r="E57">
-        <v>111</v>
-      </c>
-      <c r="F57">
         <v>56</v>
       </c>
+      <c r="F57" t="s">
+        <v>198</v>
+      </c>
       <c r="G57" t="s">
+        <v>205</v>
+      </c>
+      <c r="H57" t="s">
+        <v>210</v>
+      </c>
+      <c r="I57" t="s">
         <v>198</v>
       </c>
-      <c r="H57" t="s">
-        <v>205</v>
-      </c>
-      <c r="I57" t="s">
-        <v>210</v>
-      </c>
       <c r="J57" t="s">
-        <v>198</v>
-      </c>
-      <c r="K57" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2825,29 +2829,29 @@
       <c r="C58" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="D58">
+        <v>113</v>
+      </c>
       <c r="E58">
-        <v>113</v>
-      </c>
-      <c r="F58">
         <v>57</v>
       </c>
+      <c r="F58" t="s">
+        <v>184</v>
+      </c>
       <c r="G58" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="H58" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="I58" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J58" t="s">
-        <v>184</v>
-      </c>
-      <c r="K58" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2857,25 +2861,25 @@
       <c r="C59" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="D59">
+        <v>115</v>
+      </c>
       <c r="E59">
-        <v>115</v>
-      </c>
-      <c r="F59">
         <v>58</v>
       </c>
+      <c r="F59" t="s">
+        <v>184</v>
+      </c>
       <c r="G59" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H59" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I59" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J59" t="s">
-        <v>184</v>
-      </c>
-      <c r="K59" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>